<commit_message>
Il faut encore réflechir.
</commit_message>
<xml_diff>
--- a/Evaluation_V2/Bareme.xlsx
+++ b/Evaluation_V2/Bareme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Enseignement\GitHub\PSI\Evaluation_V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{93C96112-7253-4607-AE4F-B3FE56A3AFE7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AAECEBAA-9E4C-40AF-A628-79085782F6EF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1822,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB18" sqref="AB18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,27 +1954,27 @@
       </c>
       <c r="D2">
         <f>SUM(D3:D145)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:AJ2" si="0">SUM(E3:E145)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J2">
         <f t="shared" si="0"/>
@@ -1986,27 +1986,27 @@
       </c>
       <c r="L2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="O2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Q2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R2">
         <f t="shared" si="0"/>
@@ -2018,55 +2018,55 @@
       </c>
       <c r="T2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="V2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="W2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Y2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="Z2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AA2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="AB2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AD2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AE2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG2">
         <f t="shared" si="0"/>
@@ -2123,7 +2123,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -2162,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -2236,7 +2236,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -2275,7 +2275,7 @@
         <v>0</v>
       </c>
       <c r="AA4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB4">
         <v>0</v>
@@ -2349,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -2388,7 +2388,7 @@
         <v>0</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5">
         <v>0</v>
@@ -2462,7 +2462,7 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -2501,7 +2501,7 @@
         <v>0</v>
       </c>
       <c r="AC6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -2575,7 +2575,7 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -2590,7 +2590,7 @@
         <v>0</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -2614,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="AD7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AE7">
         <v>0</v>
@@ -2703,7 +2703,7 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -2816,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -2914,7 +2914,7 @@
         <v>0</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -2929,7 +2929,7 @@
         <v>0</v>
       </c>
       <c r="Y10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z10">
         <v>0</v>
@@ -2953,7 +2953,7 @@
         <v>0</v>
       </c>
       <c r="AG10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH10">
         <v>0</v>
@@ -3027,7 +3027,7 @@
         <v>0</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -3113,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -3265,7 +3265,7 @@
         <v>0</v>
       </c>
       <c r="AA13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB13">
         <v>0</v>
@@ -3416,7 +3416,7 @@
         <v>26</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -3443,7 +3443,7 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -3452,7 +3452,7 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -3482,7 +3482,7 @@
         <v>0</v>
       </c>
       <c r="Z15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA15">
         <v>0</v>
@@ -3529,7 +3529,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -3556,7 +3556,7 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -3565,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R16">
         <v>0</v>
@@ -3595,7 +3595,7 @@
         <v>0</v>
       </c>
       <c r="AA16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB16">
         <v>0</v>
@@ -3642,7 +3642,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -3669,7 +3669,7 @@
         <v>0</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -3678,7 +3678,7 @@
         <v>0</v>
       </c>
       <c r="R17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S17">
         <v>0</v>
@@ -3755,7 +3755,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -3782,7 +3782,7 @@
         <v>0</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -3791,7 +3791,7 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18">
         <v>0</v>
@@ -3868,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -3895,7 +3895,7 @@
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R19">
         <v>0</v>
@@ -3904,13 +3904,13 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U19">
         <v>0</v>
       </c>
       <c r="V19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W19">
         <v>0</v>
@@ -3981,7 +3981,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -4017,13 +4017,13 @@
         <v>0</v>
       </c>
       <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
         <v>1</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-      <c r="W20">
-        <v>0</v>
       </c>
       <c r="X20">
         <v>0</v>
@@ -4130,13 +4130,13 @@
         <v>0</v>
       </c>
       <c r="V21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W21">
         <v>0</v>
       </c>
       <c r="X21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y21">
         <v>0</v>
@@ -4234,7 +4234,7 @@
         <v>0</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U22">
         <v>0</v>
@@ -4243,13 +4243,13 @@
         <v>0</v>
       </c>
       <c r="W22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X22">
         <v>0</v>
       </c>
       <c r="Y22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z22">
         <v>0</v>
@@ -4320,7 +4320,7 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -4347,7 +4347,7 @@
         <v>0</v>
       </c>
       <c r="U23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V23">
         <v>0</v>
@@ -4356,7 +4356,7 @@
         <v>0</v>
       </c>
       <c r="X23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y23">
         <v>0</v>
@@ -4469,7 +4469,7 @@
         <v>0</v>
       </c>
       <c r="Y24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z24">
         <v>0</v>
@@ -4546,7 +4546,7 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -4582,13 +4582,13 @@
         <v>0</v>
       </c>
       <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+      <c r="AB25">
         <v>1</v>
-      </c>
-      <c r="AA25">
-        <v>0</v>
-      </c>
-      <c r="AB25">
-        <v>0</v>
       </c>
       <c r="AC25">
         <v>0</v>
@@ -4695,13 +4695,13 @@
         <v>0</v>
       </c>
       <c r="AA26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB26">
         <v>0</v>
       </c>
       <c r="AC26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD26">
         <v>0</v>
@@ -4772,7 +4772,7 @@
         <v>0</v>
       </c>
       <c r="P27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q27">
         <v>0</v>
@@ -4808,7 +4808,7 @@
         <v>0</v>
       </c>
       <c r="AB27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC27">
         <v>0</v>
@@ -4885,7 +4885,7 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R28">
         <v>0</v>
@@ -4900,7 +4900,7 @@
         <v>0</v>
       </c>
       <c r="V28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W28">
         <v>0</v>
@@ -4921,7 +4921,7 @@
         <v>0</v>
       </c>
       <c r="AC28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD28">
         <v>0</v>
@@ -4998,7 +4998,7 @@
         <v>0</v>
       </c>
       <c r="R29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S29">
         <v>0</v>
@@ -5034,7 +5034,7 @@
         <v>0</v>
       </c>
       <c r="AD29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE29">
         <v>0</v>
@@ -5111,7 +5111,7 @@
         <v>0</v>
       </c>
       <c r="S30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T30">
         <v>0</v>
@@ -5147,7 +5147,7 @@
         <v>0</v>
       </c>
       <c r="AE30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF30">
         <v>0</v>
@@ -5224,7 +5224,7 @@
         <v>0</v>
       </c>
       <c r="T31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U31">
         <v>0</v>
@@ -5260,7 +5260,7 @@
         <v>0</v>
       </c>
       <c r="AF31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG31">
         <v>0</v>
@@ -5337,7 +5337,7 @@
         <v>0</v>
       </c>
       <c r="U32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V32">
         <v>0</v>
@@ -5373,7 +5373,7 @@
         <v>0</v>
       </c>
       <c r="AG32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH32">
         <v>0</v>

</xml_diff>

<commit_message>
Ca marche pas encore ;(
</commit_message>
<xml_diff>
--- a/Evaluation_V2/Bareme.xlsx
+++ b/Evaluation_V2/Bareme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Enseignement\GitHub\PSI\Evaluation_V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{05DCAD84-BF3B-4585-97C3-D667A042FC2E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7186C5C-6163-4669-97D5-C4CBC65C03D1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1822,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AJ3" sqref="AJ3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:AJ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1957,23 +1957,23 @@
         <v>4</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:AJ2" si="0">SUM(E4:E146)</f>
+        <f>SUM(E4:E146)</f>
         <v>5</v>
       </c>
       <c r="F2">
-        <f t="shared" si="0"/>
+        <f>SUM(F4:F146)</f>
         <v>8</v>
       </c>
       <c r="G2">
-        <f t="shared" si="0"/>
+        <f>SUM(G4:G146)</f>
         <v>3</v>
       </c>
       <c r="H2">
-        <f t="shared" si="0"/>
+        <f>SUM(H4:H146)</f>
         <v>6</v>
       </c>
       <c r="I2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I2:AJ2" si="0">SUM(I4:I146)</f>
         <v>9</v>
       </c>
       <c r="J2">

</xml_diff>